<commit_message>
se realizó reto semanal semana 4
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianaperez/Desktop/ejercicios_trainee_bdg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64862626-7289-354A-8930-481CF0D7E55A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC3310-4118-4049-BCBA-FF94F79E5EC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="1880" windowWidth="22220" windowHeight="13380" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
     <sheet name="Semana 2" sheetId="2" r:id="rId2"/>
     <sheet name="Semana 3" sheetId="3" r:id="rId3"/>
     <sheet name="Semana 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Semana 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="24">
   <si>
     <t xml:space="preserve">SEMANA </t>
   </si>
@@ -89,6 +90,18 @@
   <si>
     <t>Reto Semanal 3</t>
   </si>
+  <si>
+    <t>RETO SEMANAL</t>
+  </si>
+  <si>
+    <t>125 Ejercicio</t>
+  </si>
+  <si>
+    <t>139 Ejercicio</t>
+  </si>
+  <si>
+    <t>DIA ENTREGA</t>
+  </si>
 </sst>
 </file>
 
@@ -125,7 +138,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,6 +311,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,25 +335,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2272,7 +2315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3109,8 +3154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3157,10 +3202,10 @@
         <v>105</v>
       </c>
       <c r="G3" s="27"/>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="24"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
@@ -3172,15 +3217,15 @@
         <v>10</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <f>F3+1</f>
         <v>106</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
@@ -3192,15 +3237,15 @@
         <v>10</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="F5" s="22">
+      <c r="F5" s="20">
         <f>F4+1</f>
         <v>107</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
@@ -3216,10 +3261,10 @@
         <v>17</v>
       </c>
       <c r="G6" s="20"/>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="17"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
@@ -3231,14 +3276,14 @@
         <v>10</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="23"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
@@ -3250,8 +3295,8 @@
         <v>3</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
     </row>
@@ -3265,8 +3310,8 @@
         <v>3</v>
       </c>
       <c r="D9" s="13"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
     </row>
@@ -3280,8 +3325,8 @@
         <v>3</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
     </row>
@@ -3295,8 +3340,8 @@
         <v>3</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
@@ -3310,50 +3355,50 @@
         <v>3</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
+      <c r="A14" s="20">
         <v>104</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="25">
+      <c r="A15" s="18">
         <f>A14+1</f>
         <v>105</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26" t="str">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19" t="str">
         <f>C14</f>
         <v>Miercoles</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -3420,4 +3465,487 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45F3675-5C35-734F-8CA2-70AF5B7D597B}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="F2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="K2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8"/>
+      <c r="M2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="27">
+        <v>109</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="F3" s="33">
+        <f>A15+1</f>
+        <v>122</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="K3" s="33">
+        <f>F15+1</f>
+        <v>135</v>
+      </c>
+      <c r="L3" s="33"/>
+      <c r="M3" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="32"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="20">
+        <f t="shared" ref="A4:A14" si="0">A3+1</f>
+        <v>110</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="F4" s="28">
+        <f t="shared" ref="F4:F14" si="1">F3+1</f>
+        <v>123</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="29"/>
+      <c r="K4" s="28">
+        <f t="shared" ref="K4:K6" si="2">K3+1</f>
+        <v>136</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="32"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="20">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="F5" s="28">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="29"/>
+      <c r="K5" s="28">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="L5" s="28"/>
+      <c r="M5" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="32"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="20">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="F6" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="29"/>
+      <c r="K6" s="28">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="L6" s="28"/>
+      <c r="M6" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="32"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="20">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="F7" s="28">
+        <f>F5+2</f>
+        <v>126</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="K7" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="28"/>
+      <c r="M7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="32"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="20">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="F8" s="28">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="K8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="34"/>
+      <c r="M8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="35"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="28">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="F9" s="28">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="28">
+        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="F10" s="28">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="28">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="F11" s="28">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="29"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="28">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="F12" s="28">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="29"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="28">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="F13" s="28">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="29"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="28">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="F14" s="28">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <f>A14+1</f>
+        <v>121</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31" t="str">
+        <f>C14</f>
+        <v>Martes</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="F15" s="30">
+        <f>F14+1</f>
+        <v>134</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31" t="str">
+        <f>H14</f>
+        <v>Jueves</v>
+      </c>
+      <c r="I15" s="31"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="85">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se finalizó semana 5
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianaperez/Desktop/ejercicios_trainee_bdg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC3310-4118-4049-BCBA-FF94F79E5EC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5992A91F-C998-3843-9FF7-FC719F0ED641}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Semana 4" sheetId="4" r:id="rId4"/>
     <sheet name="Semana 5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="25">
   <si>
     <t xml:space="preserve">SEMANA </t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>DIA ENTREGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,16 +356,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3471,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45F3675-5C35-734F-8CA2-70AF5B7D597B}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3522,24 +3522,24 @@
         <v>10</v>
       </c>
       <c r="D3" s="26"/>
-      <c r="F3" s="33">
+      <c r="F3" s="27">
         <f>A15+1</f>
         <v>122</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="29" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="K3" s="33">
+      <c r="I3" s="21"/>
+      <c r="K3" s="27">
         <f>F15+1</f>
         <v>135</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="27"/>
+      <c r="M3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="32"/>
+      <c r="N3" s="26"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
@@ -3551,24 +3551,24 @@
         <v>10</v>
       </c>
       <c r="D4" s="26"/>
-      <c r="F4" s="28">
+      <c r="F4" s="20">
         <f t="shared" ref="F4:F14" si="1">F3+1</f>
         <v>123</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="29"/>
+      <c r="I4" s="21"/>
       <c r="K4" s="28">
         <f t="shared" ref="K4:K6" si="2">K3+1</f>
         <v>136</v>
       </c>
       <c r="L4" s="28"/>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="32"/>
+      <c r="N4" s="34"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
@@ -3580,24 +3580,24 @@
         <v>10</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="F5" s="28">
+      <c r="F5" s="20">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="21"/>
       <c r="K5" s="28">
         <f t="shared" si="2"/>
         <v>137</v>
       </c>
       <c r="L5" s="28"/>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="32"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
@@ -3609,23 +3609,23 @@
         <v>10</v>
       </c>
       <c r="D6" s="26"/>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="21"/>
       <c r="K6" s="28">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="L6" s="28"/>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="32"/>
+      <c r="N6" s="34"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
@@ -3637,23 +3637,23 @@
         <v>10</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="F7" s="28">
+      <c r="F7" s="20">
         <f>F5+2</f>
         <v>126</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="29"/>
+      <c r="I7" s="21"/>
       <c r="K7" s="28" t="s">
         <v>22</v>
       </c>
       <c r="L7" s="28"/>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="32"/>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
@@ -3665,189 +3665,192 @@
         <v>10</v>
       </c>
       <c r="D8" s="26"/>
-      <c r="F8" s="28">
+      <c r="F8" s="20">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="K8" s="34" t="s">
+      <c r="I8" s="21"/>
+      <c r="K8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="34"/>
-      <c r="M8" s="35" t="s">
+      <c r="L8" s="32"/>
+      <c r="M8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="35"/>
+      <c r="N8" s="33"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="28">
+      <c r="A9" s="20">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="F9" s="28">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="F9" s="20">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="29"/>
+      <c r="I9" s="21"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
       <c r="M9" s="29"/>
       <c r="N9" s="29"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="28">
+      <c r="A10" s="20">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="F10" s="28">
+      <c r="B10" s="20"/>
+      <c r="C10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="F10" s="20">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29" t="s">
+      <c r="G10" s="20"/>
+      <c r="H10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="29"/>
+      <c r="I10" s="21"/>
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
       <c r="M10" s="29"/>
       <c r="N10" s="29"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
+      <c r="A11" s="20">
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="F11" s="28">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="20">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29" t="s">
+      <c r="G11" s="20"/>
+      <c r="H11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="29"/>
+      <c r="I11" s="21"/>
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
       <c r="M11" s="29"/>
       <c r="N11" s="29"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="28">
+      <c r="A12" s="20">
         <f t="shared" si="0"/>
         <v>118</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="F12" s="28">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="F12" s="20">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29" t="s">
+      <c r="G12" s="20"/>
+      <c r="H12" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="21"/>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
       <c r="M12" s="29"/>
       <c r="N12" s="29"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="28">
+      <c r="A13" s="20">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="F13" s="28">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="F13" s="20">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29" t="s">
+      <c r="G13" s="20"/>
+      <c r="H13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="29"/>
+      <c r="I13" s="21"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
+      <c r="A14" s="20">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="F14" s="28">
+      <c r="B14" s="20"/>
+      <c r="C14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="F14" s="20">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29" t="s">
+      <c r="G14" s="20"/>
+      <c r="H14" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="21"/>
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
       <c r="M14" s="29"/>
       <c r="N14" s="29"/>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="18">
         <f>A14+1</f>
         <v>121</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="str">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19" t="str">
         <f>C14</f>
         <v>Martes</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="F15" s="30">
+      <c r="D15" s="19"/>
+      <c r="F15" s="18">
         <f>F14+1</f>
         <v>134</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31" t="str">
+      <c r="G15" s="18"/>
+      <c r="H15" s="19" t="str">
         <f>H14</f>
         <v>Jueves</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="19"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="31"/>

</xml_diff>

<commit_message>
Se realizó reto semanal 5 y ejercicio 147
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianaperez/Desktop/ejercicios_trainee_bdg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5992A91F-C998-3843-9FF7-FC719F0ED641}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE084030-01DE-A14A-B233-81E1C6C0033C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Semana 3" sheetId="3" r:id="rId3"/>
     <sheet name="Semana 4" sheetId="4" r:id="rId4"/>
     <sheet name="Semana 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Semana 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="26">
   <si>
     <t xml:space="preserve">SEMANA </t>
   </si>
@@ -105,6 +106,9 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>147 Ejercicio</t>
+  </si>
 </sst>
 </file>
 
@@ -167,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -257,15 +261,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,6 +394,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -760,672 +797,672 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="10"/>
+      <c r="K2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="F3" s="3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="4">
         <v>13</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="K3" s="3">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="K3" s="4">
         <v>25</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="F4" s="3">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="4">
         <v>14</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="K4" s="3">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="K4" s="4">
         <v>26</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="3">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="4">
         <v>15</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="K5" s="3" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="K5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="3">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="4">
         <v>16</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="K6" s="3">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="K6" s="4">
         <v>27</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="F7" s="4">
         <v>17</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="K7" s="3" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="K7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="F8" s="4">
         <v>18</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="K8" s="3">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="K8" s="4">
         <v>29</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="F9" s="3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="F9" s="4">
         <v>19</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="K9" s="3">
+      <c r="G9" s="4"/>
+      <c r="H9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="K9" s="4">
         <v>30</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="F10" s="3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="4">
         <v>20</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="K10" s="3">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="K10" s="4">
         <v>31</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4" t="s">
+      <c r="L10" s="4"/>
+      <c r="M10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="F11" s="3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="F11" s="4">
         <v>21</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="K11" s="3">
+      <c r="G11" s="4"/>
+      <c r="H11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="K11" s="4">
         <v>32</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="4" t="s">
+      <c r="L11" s="4"/>
+      <c r="M11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="F12" s="3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="F12" s="4">
         <v>22</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="K12" s="3">
+      <c r="G12" s="4"/>
+      <c r="H12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="K12" s="4">
         <v>33</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="4" t="s">
+      <c r="L12" s="4"/>
+      <c r="M12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="F13" s="3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="F13" s="4">
         <v>23</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="4"/>
-      <c r="K13" s="3">
+      <c r="G13" s="4"/>
+      <c r="H13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="K13" s="4">
         <v>34</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="4" t="s">
+      <c r="L13" s="4"/>
+      <c r="M13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="F14" s="5">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="F14" s="6">
         <v>24</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="6"/>
-      <c r="K14" s="3">
+      <c r="G14" s="6"/>
+      <c r="H14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="K14" s="4">
         <v>35</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="4" t="s">
+      <c r="L14" s="4"/>
+      <c r="M14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="K15" s="3">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="K15" s="4">
         <v>36</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="4" t="s">
+      <c r="L15" s="4"/>
+      <c r="M15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N15" s="4"/>
+      <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="K16" s="3">
+      <c r="K16" s="4">
         <v>37</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="4" t="s">
+      <c r="L16" s="4"/>
+      <c r="M16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="4"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="11:14" x14ac:dyDescent="0.2">
-      <c r="K17" s="5">
+      <c r="K17" s="6">
         <v>38</v>
       </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6" t="s">
+      <c r="L17" s="6"/>
+      <c r="M17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="6"/>
+      <c r="N17" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="181">
@@ -1630,531 +1667,531 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>39</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="F3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>40</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="F4" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>41</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="4">
         <v>52</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>42</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="4">
         <v>53</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>43</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="F7" s="4">
         <v>54</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>44</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="F8" s="4">
         <v>55</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>45</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="F9" s="10">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="F9" s="11">
         <v>56</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>46</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="F10" s="3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="4">
         <v>57</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>47</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="F11" s="3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="F11" s="4">
         <v>58</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>48</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="F12" s="3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="F12" s="4">
         <v>59</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>49</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="F13" s="3" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="6">
         <f>A13+1</f>
         <v>50</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="F14" s="5" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="F14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="147">
@@ -2326,646 +2363,646 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="10"/>
+      <c r="K2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>61</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="F3" s="3">
+      <c r="D3" s="5"/>
+      <c r="F3" s="4">
         <v>73</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="K3" s="3">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="K3" s="4">
         <v>85</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="4"/>
+      <c r="M3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <v>62</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="F4" s="3">
+      <c r="D4" s="5"/>
+      <c r="F4" s="4">
         <v>74</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="K4" s="3">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="K4" s="4">
         <v>86</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="4" t="s">
+      <c r="L4" s="4"/>
+      <c r="M4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="13">
         <v>63</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="3">
+      <c r="D5" s="5"/>
+      <c r="F5" s="4">
         <v>75</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="K5" s="3">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="K5" s="4">
         <v>87</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="4" t="s">
+      <c r="L5" s="4"/>
+      <c r="M5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>64</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="5"/>
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="K6" s="3">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="K6" s="4">
         <v>88</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="4" t="s">
+      <c r="L6" s="4"/>
+      <c r="M6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="13">
         <v>65</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="F7" s="3">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="F7" s="4">
         <v>77</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="K7" s="3">
+      <c r="G7" s="4"/>
+      <c r="H7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="K7" s="4">
         <v>89</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="4" t="s">
+      <c r="L7" s="4"/>
+      <c r="M7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <v>66</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="F8" s="3">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="F8" s="4">
         <v>78</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="K8" s="3">
+      <c r="G8" s="4"/>
+      <c r="H8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="K8" s="4">
         <v>90</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4" t="s">
+      <c r="L8" s="4"/>
+      <c r="M8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <v>67</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="F9" s="3">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="F9" s="4">
         <v>79</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="K9" s="3">
+      <c r="G9" s="4"/>
+      <c r="H9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="K9" s="4">
         <v>91</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4" t="s">
+      <c r="L9" s="4"/>
+      <c r="M9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="F10" s="3">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="F10" s="4">
         <v>80</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="K10" s="3">
+      <c r="G10" s="4"/>
+      <c r="H10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="K10" s="4">
         <v>92</v>
       </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4" t="s">
+      <c r="L10" s="4"/>
+      <c r="M10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="F11" s="3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="F11" s="4">
         <v>81</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="K11" s="16" t="s">
+      <c r="G11" s="4"/>
+      <c r="H11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="K11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="17" t="s">
+      <c r="L11" s="17"/>
+      <c r="M11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="17"/>
+      <c r="N11" s="18"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>69</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="F12" s="3">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="F12" s="4">
         <v>82</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="K12" s="16" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="K12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17" t="s">
+      <c r="L12" s="17"/>
+      <c r="M12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="17"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>70</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="F13" s="3">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="F13" s="4">
         <v>83</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="K13" s="16" t="s">
+      <c r="I13" s="5"/>
+      <c r="K13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17" t="s">
+      <c r="L13" s="17"/>
+      <c r="M13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="17"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>71</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="F14" s="5">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="F14" s="6">
         <f>F13+1</f>
         <v>84</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="K14" s="14" t="s">
+      <c r="I14" s="7"/>
+      <c r="K14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="16"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <f>A14+1</f>
         <v>72</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="175">
@@ -3161,244 +3198,244 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>93</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="F3" s="27">
+      <c r="D3" s="5"/>
+      <c r="F3" s="28">
         <f>A15</f>
         <v>105</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>94</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="F4" s="20">
+      <c r="D4" s="5"/>
+      <c r="F4" s="21">
         <f>F3+1</f>
         <v>106</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="26"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="13">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="F5" s="20">
+      <c r="D5" s="14"/>
+      <c r="F5" s="21">
         <f>F4+1</f>
         <v>107</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="F6" s="20" t="s">
+      <c r="D6" s="5"/>
+      <c r="F6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="21"/>
+      <c r="H6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="26"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="13">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="20" t="s">
+      <c r="D7" s="5"/>
+      <c r="F7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="26" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="26"/>
+      <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="13">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
+      <c r="A10" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
+      <c r="A11" s="13">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="D13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="A14" s="21">
         <v>104</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="D14" s="22"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="18">
+      <c r="A15" s="19">
         <f>A14+1</f>
         <v>105</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="str">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20" t="str">
         <f>C14</f>
         <v>Miercoles</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -3471,390 +3508,390 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45F3675-5C35-734F-8CA2-70AF5B7D597B}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="10"/>
+      <c r="K2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="27">
+      <c r="A3" s="28">
         <v>109</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="F3" s="27">
+      <c r="D3" s="27"/>
+      <c r="F3" s="28">
         <f>A15+1</f>
         <v>122</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="K3" s="27">
+      <c r="I3" s="22"/>
+      <c r="K3" s="28">
         <f>F15+1</f>
         <v>135</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="26" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="26"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
+      <c r="A4" s="21">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>110</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="F4" s="20">
+      <c r="D4" s="27"/>
+      <c r="F4" s="21">
         <f t="shared" ref="F4:F14" si="1">F3+1</f>
         <v>123</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="K4" s="28">
+      <c r="I4" s="22"/>
+      <c r="K4" s="21">
         <f t="shared" ref="K4:K6" si="2">K3+1</f>
         <v>136</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="34" t="s">
+      <c r="L4" s="21"/>
+      <c r="M4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="34"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="A5" s="21">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="F5" s="20">
+      <c r="D5" s="22"/>
+      <c r="F5" s="21">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21" t="s">
+      <c r="G5" s="21"/>
+      <c r="H5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="K5" s="28">
+      <c r="I5" s="22"/>
+      <c r="K5" s="21">
         <f t="shared" si="2"/>
         <v>137</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="34" t="s">
+      <c r="L5" s="21"/>
+      <c r="M5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="34"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="A6" s="21">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="F6" s="20" t="s">
+      <c r="D6" s="27"/>
+      <c r="F6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21" t="s">
+      <c r="G6" s="21"/>
+      <c r="H6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="K6" s="28">
+      <c r="I6" s="22"/>
+      <c r="K6" s="21">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="34" t="s">
+      <c r="L6" s="21"/>
+      <c r="M6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
+      <c r="A7" s="21">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="F7" s="20">
+      <c r="D7" s="27"/>
+      <c r="F7" s="21">
         <f>F5+2</f>
         <v>126</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="K7" s="28" t="s">
+      <c r="I7" s="22"/>
+      <c r="K7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="28"/>
-      <c r="M7" s="34" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="34"/>
+      <c r="N7" s="27"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="F8" s="20">
+      <c r="D8" s="27"/>
+      <c r="F8" s="21">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="K8" s="32" t="s">
+      <c r="I8" s="22"/>
+      <c r="K8" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="33" t="s">
+      <c r="L8" s="33"/>
+      <c r="M8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="33"/>
+      <c r="N8" s="34"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="F9" s="20">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="F9" s="21">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
+      <c r="I9" s="22"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="F10" s="20">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="F10" s="21">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
+      <c r="I10" s="22"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="20">
+      <c r="A11" s="21">
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="22"/>
       <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="21">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
+      <c r="I11" s="22"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="A12" s="21">
         <f t="shared" si="0"/>
         <v>118</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="F12" s="20">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="F12" s="21">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21" t="s">
+      <c r="G12" s="21"/>
+      <c r="H12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
+      <c r="I12" s="22"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
+      <c r="A13" s="21">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="F13" s="20">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="F13" s="21">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
+      <c r="I13" s="22"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="A14" s="21">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="F14" s="20">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="F14" s="21">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21" t="s">
+      <c r="G14" s="21"/>
+      <c r="H14" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
+      <c r="I14" s="22"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="19">
         <f>A14+1</f>
         <v>121</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19" t="str">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20" t="str">
         <f>C14</f>
         <v>Martes</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="F15" s="18">
+      <c r="D15" s="20"/>
+      <c r="F15" s="19">
         <f>F14+1</f>
         <v>134</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19" t="str">
+      <c r="G15" s="19"/>
+      <c r="H15" s="20" t="str">
         <f>H14</f>
         <v>Jueves</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
+      <c r="I15" s="20"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="85">
@@ -3951,4 +3988,382 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB16AC32-C8EA-8643-BBE4-B1CA4CCBF32F}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="28">
+        <v>140</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="28">
+        <f>A15+1</f>
+        <v>153</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="27"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <f t="shared" ref="A4:A14" si="0">A3+1</f>
+        <v>141</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="21">
+        <f t="shared" ref="F4:F11" si="1">F3+1</f>
+        <v>154</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="27"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="29">
+        <f t="shared" si="1"/>
+        <v>155</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="35"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="29">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="29">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="29">
+        <f t="shared" si="1"/>
+        <v>158</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="21">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="29">
+        <f t="shared" si="1"/>
+        <v>159</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="35"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="29">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="21">
+        <f>A9+2</f>
+        <v>148</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="27"/>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="29">
+        <f t="shared" si="1"/>
+        <v>161</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="35"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="27"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <f>A14+1</f>
+        <v>152</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="36" t="str">
+        <f>C14</f>
+        <v>Jueves</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="57">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se implemento busqueda en el reto semanal
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianaperez/Desktop/ejercicios_trainee_bdg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE084030-01DE-A14A-B233-81E1C6C0033C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61074F10-B79F-744B-BB3C-6AA35F0BA9F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Semana 4" sheetId="4" r:id="rId4"/>
     <sheet name="Semana 5" sheetId="5" r:id="rId5"/>
     <sheet name="Semana 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Semana 7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="27">
   <si>
     <t xml:space="preserve">SEMANA </t>
   </si>
@@ -108,6 +109,9 @@
   </si>
   <si>
     <t>147 Ejercicio</t>
+  </si>
+  <si>
+    <t>Reto Semanal Pasado</t>
   </si>
 </sst>
 </file>
@@ -291,12 +295,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,13 +400,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -797,672 +822,672 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="9" t="s">
+      <c r="I2" s="11"/>
+      <c r="K2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="F3" s="4">
+      <c r="D3" s="6"/>
+      <c r="F3" s="5">
         <v>13</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="K3" s="4">
+      <c r="I3" s="6"/>
+      <c r="K3" s="5">
         <v>25</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="F4" s="4">
+      <c r="D4" s="6"/>
+      <c r="F4" s="5">
         <v>14</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="K4" s="4">
+      <c r="I4" s="6"/>
+      <c r="K4" s="5">
         <v>26</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="F5" s="4">
+      <c r="D5" s="6"/>
+      <c r="F5" s="5">
         <v>15</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="K5" s="4" t="s">
+      <c r="I5" s="6"/>
+      <c r="K5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="F6" s="4">
+      <c r="D6" s="6"/>
+      <c r="F6" s="5">
         <v>16</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="K6" s="4">
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="5">
         <v>27</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="F7" s="4">
+      <c r="D7" s="6"/>
+      <c r="F7" s="5">
         <v>17</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="4" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="K7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="F8" s="4">
+      <c r="D8" s="6"/>
+      <c r="F8" s="5">
         <v>18</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="K8" s="4">
+      <c r="G8" s="5"/>
+      <c r="H8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="K8" s="5">
         <v>29</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="F9" s="4">
+      <c r="D9" s="6"/>
+      <c r="F9" s="5">
         <v>19</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="K9" s="4">
+      <c r="G9" s="5"/>
+      <c r="H9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="K9" s="5">
         <v>30</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="F10" s="4">
+      <c r="D10" s="6"/>
+      <c r="F10" s="5">
         <v>20</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="K10" s="4">
+      <c r="G10" s="5"/>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="K10" s="5">
         <v>31</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="5"/>
+      <c r="M10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="5"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="F11" s="4">
+      <c r="D11" s="6"/>
+      <c r="F11" s="5">
         <v>21</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="K11" s="4">
+      <c r="G11" s="5"/>
+      <c r="H11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="K11" s="5">
         <v>32</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="5" t="s">
+      <c r="L11" s="5"/>
+      <c r="M11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="5"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="F12" s="4">
+      <c r="D12" s="6"/>
+      <c r="F12" s="5">
         <v>22</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="K12" s="4">
+      <c r="G12" s="5"/>
+      <c r="H12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="K12" s="5">
         <v>33</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5" t="s">
+      <c r="L12" s="5"/>
+      <c r="M12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="5"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="F13" s="4">
+      <c r="D13" s="6"/>
+      <c r="F13" s="5">
         <v>23</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="5"/>
-      <c r="K13" s="4">
+      <c r="G13" s="5"/>
+      <c r="H13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="K13" s="5">
         <v>34</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5" t="s">
+      <c r="L13" s="5"/>
+      <c r="M13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="5"/>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="F14" s="6">
+      <c r="D14" s="6"/>
+      <c r="F14" s="7">
         <v>24</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="K14" s="4">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="K14" s="5">
         <v>35</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="5" t="s">
+      <c r="L14" s="5"/>
+      <c r="M14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="5"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <v>12</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="K15" s="4">
+      <c r="D15" s="8"/>
+      <c r="K15" s="5">
         <v>36</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="5" t="s">
+      <c r="L15" s="5"/>
+      <c r="M15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N15" s="5"/>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="K16" s="4">
+      <c r="K16" s="5">
         <v>37</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="5" t="s">
+      <c r="L16" s="5"/>
+      <c r="M16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="5"/>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" spans="11:14" x14ac:dyDescent="0.2">
-      <c r="K17" s="6">
+      <c r="K17" s="7">
         <v>38</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="7" t="s">
+      <c r="L17" s="7"/>
+      <c r="M17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="7"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="181">
@@ -1667,531 +1692,531 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>39</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="6"/>
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>40</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="F4" s="4" t="s">
+      <c r="D4" s="6"/>
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>41</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="F5" s="4">
+      <c r="D5" s="6"/>
+      <c r="F5" s="5">
         <v>52</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <v>42</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="F6" s="4">
+      <c r="D6" s="6"/>
+      <c r="F6" s="5">
         <v>53</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>43</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="F7" s="4">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="F7" s="5">
         <v>54</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>44</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="F8" s="4">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="F8" s="5">
         <v>55</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <v>45</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="F9" s="11">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="F9" s="12">
         <v>56</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>46</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="F10" s="4">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="F10" s="5">
         <v>57</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>47</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="F11" s="4">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="F11" s="5">
         <v>58</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>48</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="F12" s="4">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="F12" s="5">
         <v>59</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <v>49</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="F13" s="4" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="F13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <f>A13+1</f>
         <v>50</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="F14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="F14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="147">
@@ -2363,646 +2388,646 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="9" t="s">
+      <c r="I2" s="11"/>
+      <c r="K2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>61</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="F3" s="4">
+      <c r="D3" s="6"/>
+      <c r="F3" s="5">
         <v>73</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="K3" s="4">
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="K3" s="5">
         <v>85</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="5"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>62</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="F4" s="4">
+      <c r="D4" s="6"/>
+      <c r="F4" s="5">
         <v>74</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="K4" s="4">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="K4" s="5">
         <v>86</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="5"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <v>63</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="F5" s="4">
+      <c r="D5" s="6"/>
+      <c r="F5" s="5">
         <v>75</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="K5" s="4">
+      <c r="G5" s="5"/>
+      <c r="H5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="K5" s="5">
         <v>87</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5" t="s">
+      <c r="L5" s="5"/>
+      <c r="M5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="5"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <v>64</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="6"/>
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="K6" s="4">
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="5">
         <v>88</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="5"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+      <c r="A7" s="14">
         <v>65</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="F7" s="4">
+      <c r="D7" s="15"/>
+      <c r="F7" s="5">
         <v>77</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="4">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="K7" s="5">
         <v>89</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5" t="s">
+      <c r="L7" s="5"/>
+      <c r="M7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="5"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <v>66</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="F8" s="4">
+      <c r="D8" s="15"/>
+      <c r="F8" s="5">
         <v>78</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="K8" s="4">
+      <c r="G8" s="5"/>
+      <c r="H8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="K8" s="5">
         <v>90</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5" t="s">
+      <c r="L8" s="5"/>
+      <c r="M8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="5"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <v>67</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="F9" s="4">
+      <c r="D9" s="15"/>
+      <c r="F9" s="5">
         <v>79</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="K9" s="4">
+      <c r="G9" s="5"/>
+      <c r="H9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="K9" s="5">
         <v>91</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5" t="s">
+      <c r="L9" s="5"/>
+      <c r="M9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="5"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="F10" s="4">
+      <c r="D10" s="15"/>
+      <c r="F10" s="5">
         <v>80</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="K10" s="4">
+      <c r="G10" s="5"/>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="K10" s="5">
         <v>92</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5" t="s">
+      <c r="L10" s="5"/>
+      <c r="M10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="5"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="F11" s="4">
+      <c r="D11" s="15"/>
+      <c r="F11" s="5">
         <v>81</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="K11" s="17" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="K11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="18"/>
+      <c r="M11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="18"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <v>69</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="F12" s="4">
+      <c r="D12" s="15"/>
+      <c r="F12" s="5">
         <v>82</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="K12" s="17" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="K12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="18" t="s">
+      <c r="L12" s="18"/>
+      <c r="M12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="18"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+      <c r="A13" s="14">
         <v>70</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="F13" s="4">
+      <c r="D13" s="15"/>
+      <c r="F13" s="5">
         <v>83</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="K13" s="17" t="s">
+      <c r="I13" s="6"/>
+      <c r="K13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="18" t="s">
+      <c r="L13" s="18"/>
+      <c r="M13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="N13" s="18"/>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
+      <c r="A14" s="14">
         <v>71</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="F14" s="6">
+      <c r="D14" s="15"/>
+      <c r="F14" s="7">
         <f>F13+1</f>
         <v>84</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="K14" s="15" t="s">
+      <c r="I14" s="8"/>
+      <c r="K14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="16" t="s">
+      <c r="L14" s="16"/>
+      <c r="M14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="16"/>
+      <c r="N14" s="17"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <f>A14+1</f>
         <v>72</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="175">
@@ -3198,244 +3223,244 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>93</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="F3" s="28">
+      <c r="D3" s="6"/>
+      <c r="F3" s="29">
         <f>A15</f>
         <v>105</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="22" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="22"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>94</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="F4" s="21">
+      <c r="D4" s="6"/>
+      <c r="F4" s="22">
         <f>F3+1</f>
         <v>106</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="27" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="27"/>
+      <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
+      <c r="A5" s="14">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="F5" s="21">
+      <c r="D5" s="15"/>
+      <c r="F5" s="22">
         <f>F4+1</f>
         <v>107</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="27" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="27"/>
+      <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="F6" s="21" t="s">
+      <c r="D6" s="6"/>
+      <c r="F6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="27" t="s">
+      <c r="G6" s="22"/>
+      <c r="H6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+      <c r="A7" s="14">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="F7" s="21" t="s">
+      <c r="D7" s="6"/>
+      <c r="F7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="27" t="s">
+      <c r="G7" s="22"/>
+      <c r="H7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="27"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+      <c r="A8" s="14">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
+      <c r="A9" s="14">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="D10" s="15"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
+      <c r="A11" s="14">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="D11" s="15"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
+      <c r="A12" s="14">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="D12" s="15"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="D13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+      <c r="A14" s="22">
         <v>104</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+      <c r="D14" s="23"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
+      <c r="A15" s="20">
         <f>A14+1</f>
         <v>105</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20" t="str">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21" t="str">
         <f>C14</f>
         <v>Miercoles</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -3515,383 +3540,383 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="9" t="s">
+      <c r="I2" s="11"/>
+      <c r="K2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="28">
+      <c r="A3" s="29">
         <v>109</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="F3" s="28">
+      <c r="D3" s="28"/>
+      <c r="F3" s="29">
         <f>A15+1</f>
         <v>122</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="22" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="K3" s="28">
+      <c r="I3" s="23"/>
+      <c r="K3" s="29">
         <f>F15+1</f>
         <v>135</v>
       </c>
-      <c r="L3" s="28"/>
-      <c r="M3" s="27" t="s">
+      <c r="L3" s="29"/>
+      <c r="M3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="27"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
+      <c r="A4" s="22">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>110</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="F4" s="21">
+      <c r="D4" s="28"/>
+      <c r="F4" s="22">
         <f t="shared" ref="F4:F14" si="1">F3+1</f>
         <v>123</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="22"/>
-      <c r="K4" s="21">
+      <c r="I4" s="23"/>
+      <c r="K4" s="22">
         <f t="shared" ref="K4:K6" si="2">K3+1</f>
         <v>136</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="27" t="s">
+      <c r="L4" s="22"/>
+      <c r="M4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="27"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="21">
+      <c r="A5" s="22">
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="F5" s="21">
+      <c r="D5" s="23"/>
+      <c r="F5" s="22">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="K5" s="21">
+      <c r="I5" s="23"/>
+      <c r="K5" s="22">
         <f t="shared" si="2"/>
         <v>137</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="27" t="s">
+      <c r="L5" s="22"/>
+      <c r="M5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="27"/>
+      <c r="N5" s="28"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="21">
+      <c r="A6" s="22">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="F6" s="21" t="s">
+      <c r="D6" s="28"/>
+      <c r="F6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22" t="s">
+      <c r="G6" s="22"/>
+      <c r="H6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="K6" s="21">
+      <c r="I6" s="23"/>
+      <c r="K6" s="22">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="27" t="s">
+      <c r="L6" s="22"/>
+      <c r="M6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="27"/>
+      <c r="N6" s="28"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+      <c r="A7" s="22">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="F7" s="21">
+      <c r="D7" s="28"/>
+      <c r="F7" s="22">
         <f>F5+2</f>
         <v>126</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="22"/>
+      <c r="H7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="K7" s="21" t="s">
+      <c r="I7" s="23"/>
+      <c r="K7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="21"/>
-      <c r="M7" s="27" t="s">
+      <c r="L7" s="22"/>
+      <c r="M7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="27"/>
+      <c r="N7" s="28"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
+      <c r="A8" s="22">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="F8" s="21">
+      <c r="D8" s="28"/>
+      <c r="F8" s="22">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="K8" s="33" t="s">
+      <c r="I8" s="23"/>
+      <c r="K8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="33"/>
-      <c r="M8" s="34" t="s">
+      <c r="L8" s="34"/>
+      <c r="M8" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="34"/>
+      <c r="N8" s="35"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="21">
+      <c r="A9" s="22">
         <f t="shared" si="0"/>
         <v>115</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="F9" s="21">
+      <c r="D9" s="23"/>
+      <c r="F9" s="22">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
+      <c r="I9" s="23"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
+      <c r="A10" s="22">
         <f t="shared" si="0"/>
         <v>116</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="F10" s="21">
+      <c r="D10" s="23"/>
+      <c r="F10" s="22">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
+      <c r="I10" s="23"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="21">
+      <c r="A11" s="22">
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="23"/>
       <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="22">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
+      <c r="I11" s="23"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
+      <c r="A12" s="22">
         <f t="shared" si="0"/>
         <v>118</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="F12" s="21">
+      <c r="D12" s="23"/>
+      <c r="F12" s="22">
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22" t="s">
+      <c r="G12" s="22"/>
+      <c r="H12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
+      <c r="I12" s="23"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+      <c r="A13" s="22">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="F13" s="21">
+      <c r="D13" s="23"/>
+      <c r="F13" s="22">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
+      <c r="I13" s="23"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+      <c r="A14" s="22">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="F14" s="21">
+      <c r="D14" s="23"/>
+      <c r="F14" s="22">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22" t="s">
+      <c r="G14" s="22"/>
+      <c r="H14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
+      <c r="I14" s="23"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="20">
         <f>A14+1</f>
         <v>121</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20" t="str">
+      <c r="B15" s="20"/>
+      <c r="C15" s="21" t="str">
         <f>C14</f>
         <v>Martes</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="F15" s="19">
+      <c r="D15" s="21"/>
+      <c r="F15" s="20">
         <f>F14+1</f>
         <v>134</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="20" t="str">
+      <c r="G15" s="20"/>
+      <c r="H15" s="21" t="str">
         <f>H14</f>
         <v>Jueves</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="I15" s="21"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="85">
@@ -3992,311 +4017,314 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB16AC32-C8EA-8643-BBE4-B1CA4CCBF32F}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A2" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="28">
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
         <v>140</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="28">
+      <c r="F3" s="29">
         <f>A15+1</f>
         <v>153</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="27" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="27"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>141</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="21">
+      <c r="F4" s="22">
         <f t="shared" ref="F4:F11" si="1">F3+1</f>
         <v>154</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="27" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="27"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="21">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="29">
+      <c r="F5" s="22">
         <f t="shared" si="1"/>
         <v>155</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="35" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="21">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
         <f t="shared" si="0"/>
         <v>143</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="27"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="28"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="29">
+      <c r="F6" s="22">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="35" t="s">
+      <c r="G6" s="22"/>
+      <c r="H6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="22">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="27"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="29">
+      <c r="F7" s="22">
         <f t="shared" si="1"/>
         <v>157</v>
       </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="35" t="s">
+      <c r="G7" s="22"/>
+      <c r="H7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="35"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="22">
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="27"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="28"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="29">
+      <c r="F8" s="22">
         <f t="shared" si="1"/>
         <v>158</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="35" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="35"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="21">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="22">
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="27"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="28"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="29">
+      <c r="F9" s="22">
         <f t="shared" si="1"/>
         <v>159</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="35" t="s">
+      <c r="G9" s="22"/>
+      <c r="H9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="35"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="K9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="27"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="28"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="29">
+      <c r="F10" s="22">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="35" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="35"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="21">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="22">
         <f>A9+2</f>
         <v>148</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="22">
         <f t="shared" si="1"/>
         <v>161</v>
       </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="35" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="35"/>
+      <c r="I11" s="28"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="22">
         <f t="shared" si="0"/>
         <v>149</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="27" t="s">
+      <c r="G12" s="22"/>
+      <c r="H12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="27"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="22">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="27" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
         <f t="shared" si="0"/>
         <v>151</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="27" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+    <row r="15" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
         <f>A14+1</f>
         <v>152</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="36" t="str">
         <f>C14</f>
         <v>Jueves</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
       <c r="J15" s="2"/>
     </row>
   </sheetData>
@@ -4366,4 +4394,515 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9028B0E-1B65-4B46-BBD7-5B821708C0D1}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.1640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="F2" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="42"/>
+      <c r="K2" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="41"/>
+      <c r="M2" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="42"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>162</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="F3" s="29">
+        <f>A15+1</f>
+        <v>175</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="K3" s="38">
+        <f>F15+1</f>
+        <v>188</v>
+      </c>
+      <c r="L3" s="38"/>
+      <c r="M3" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="39"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <f t="shared" ref="A4:A14" si="0">A3+1</f>
+        <v>163</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="F4" s="22">
+        <f t="shared" ref="F4:F14" si="1">F3+1</f>
+        <v>176</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="K4" s="30">
+        <f t="shared" ref="K4:K11" si="2">K3+1</f>
+        <v>189</v>
+      </c>
+      <c r="L4" s="30"/>
+      <c r="M4" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="39"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="F5" s="22">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="K5" s="30">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="L5" s="30"/>
+      <c r="M5" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="39"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="F6" s="22">
+        <f t="shared" si="1"/>
+        <v>178</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="K6" s="30">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="L6" s="30"/>
+      <c r="M6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="39"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="22">
+        <f t="shared" si="0"/>
+        <v>166</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="F7" s="22">
+        <f t="shared" si="1"/>
+        <v>179</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="K7" s="30">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="L7" s="30"/>
+      <c r="M7" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="39"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="22">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="F8" s="22">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="K8" s="30">
+        <f t="shared" si="2"/>
+        <v>193</v>
+      </c>
+      <c r="L8" s="30"/>
+      <c r="M8" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="39"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="22">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="F9" s="22">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="K9" s="30">
+        <f t="shared" si="2"/>
+        <v>194</v>
+      </c>
+      <c r="L9" s="30"/>
+      <c r="M9" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="39"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="22">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="F10" s="22">
+        <f t="shared" si="1"/>
+        <v>182</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="K10" s="30">
+        <f t="shared" si="2"/>
+        <v>195</v>
+      </c>
+      <c r="L10" s="30"/>
+      <c r="M10" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="39"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="22">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="30">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="K11" s="30">
+        <f t="shared" si="2"/>
+        <v>196</v>
+      </c>
+      <c r="L11" s="30"/>
+      <c r="M11" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="39"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="22">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="F12" s="30">
+        <f t="shared" si="1"/>
+        <v>184</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="K12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="30"/>
+      <c r="M12" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="39"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="22">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="F13" s="30">
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
+        <f t="shared" si="0"/>
+        <v>173</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="F14" s="30">
+        <f t="shared" si="1"/>
+        <v>186</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="39"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <f>A14+1</f>
+        <v>174</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="36" t="str">
+        <f>C14</f>
+        <v>Jueves</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="F15" s="32">
+        <f>F14+1</f>
+        <v>187</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="43" t="str">
+        <f>H14</f>
+        <v>Viernes</v>
+      </c>
+      <c r="I15" s="44"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="85">
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se realizó último Reto semanal
</commit_message>
<xml_diff>
--- a/Planificación.xlsx
+++ b/Planificación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianaperez/Desktop/ejercicios_trainee_bdg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4638BBD4-9A57-9241-9E05-5C566ADD800A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5D0E94-9978-2142-A77E-EA2C9010D7F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15700" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Semana 6" sheetId="6" r:id="rId6"/>
     <sheet name="Semana 7" sheetId="8" r:id="rId7"/>
     <sheet name="Semana 8" sheetId="9" r:id="rId8"/>
+    <sheet name="Semana 9" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="28">
   <si>
     <t xml:space="preserve">SEMANA </t>
   </si>
@@ -153,7 +154,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +176,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -451,13 +458,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4942,10 +4961,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7116538-B24C-7348-80A7-9D2198F22B58}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:N15"/>
+    <sheetView topLeftCell="I1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4953,7 +4972,7 @@
     <col min="1" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="35" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" ht="35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -4963,7 +4982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
@@ -4988,8 +5007,16 @@
         <v>23</v>
       </c>
       <c r="N2" s="40"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="40"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <v>197</v>
       </c>
@@ -5016,8 +5043,17 @@
         <v>7</v>
       </c>
       <c r="N3" s="28"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3" s="29">
+        <f>K15+1</f>
+        <v>236</v>
+      </c>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="28"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="22">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>198</v>
@@ -5037,7 +5073,7 @@
       </c>
       <c r="I4" s="28"/>
       <c r="K4" s="22">
-        <f t="shared" ref="K4:K13" si="2">K3+1</f>
+        <f t="shared" ref="K4:K14" si="2">K3+1</f>
         <v>224</v>
       </c>
       <c r="L4" s="22"/>
@@ -5045,8 +5081,17 @@
         <v>7</v>
       </c>
       <c r="N4" s="28"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P4" s="22">
+        <f t="shared" ref="P4:P13" si="3">P3+1</f>
+        <v>237</v>
+      </c>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="28"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="22">
         <f t="shared" si="0"/>
         <v>199</v>
@@ -5070,12 +5115,21 @@
         <v>225</v>
       </c>
       <c r="L5" s="22"/>
-      <c r="M5" s="43" t="s">
+      <c r="M5" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="44"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N5" s="45"/>
+      <c r="P5" s="22">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="45"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="22">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -5099,12 +5153,21 @@
         <v>226</v>
       </c>
       <c r="L6" s="22"/>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="44"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N6" s="45"/>
+      <c r="P6" s="22">
+        <f t="shared" si="3"/>
+        <v>239</v>
+      </c>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="45"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="22">
         <f t="shared" si="0"/>
         <v>201</v>
@@ -5132,8 +5195,17 @@
         <v>14</v>
       </c>
       <c r="N7" s="28"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P7" s="22">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" s="28"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <f t="shared" si="0"/>
         <v>202</v>
@@ -5161,8 +5233,17 @@
         <v>14</v>
       </c>
       <c r="N8" s="28"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P8" s="22">
+        <f t="shared" si="3"/>
+        <v>241</v>
+      </c>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" s="28"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <f t="shared" si="0"/>
         <v>203</v>
@@ -5190,8 +5271,12 @@
         <v>14</v>
       </c>
       <c r="N9" s="28"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <f t="shared" si="0"/>
         <v>204</v>
@@ -5219,8 +5304,12 @@
         <v>14</v>
       </c>
       <c r="N10" s="28"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <f t="shared" si="0"/>
         <v>205</v>
@@ -5251,8 +5340,12 @@
         <v>14</v>
       </c>
       <c r="N11" s="28"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="46"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <f t="shared" si="0"/>
         <v>206</v>
@@ -5280,8 +5373,12 @@
         <v>14</v>
       </c>
       <c r="N12" s="28"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <f t="shared" si="0"/>
         <v>207</v>
@@ -5309,8 +5406,12 @@
         <v>14</v>
       </c>
       <c r="N13" s="28"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="46"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <f t="shared" si="0"/>
         <v>208</v>
@@ -5329,12 +5430,21 @@
         <v>7</v>
       </c>
       <c r="I14" s="28"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-    </row>
-    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="22">
+        <f t="shared" si="2"/>
+        <v>234</v>
+      </c>
+      <c r="L14" s="22"/>
+      <c r="M14" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="28"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+    </row>
+    <row r="15" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <f>A14+1</f>
         <v>209</v>
@@ -5345,27 +5455,64 @@
         <v>Miércoles</v>
       </c>
       <c r="D15" s="37"/>
-      <c r="F15" s="45">
+      <c r="F15" s="43">
         <f>F14+1</f>
         <v>222</v>
       </c>
-      <c r="G15" s="45"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="36" t="str">
         <f>H14</f>
         <v>Jueves</v>
       </c>
       <c r="I15" s="37"/>
-      <c r="K15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" s="20"/>
+      <c r="K15" s="43">
+        <f>K14+1</f>
+        <v>235</v>
+      </c>
+      <c r="L15" s="43"/>
       <c r="M15" s="36" t="s">
         <v>14</v>
       </c>
       <c r="N15" s="37"/>
+      <c r="P15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="S15" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="113">
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -5459,4 +5606,217 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4534F25C-D68E-F94A-B9FB-435045509653}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9.1640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>244</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <f t="shared" ref="A4:A13" si="0">A3+1</f>
+        <v>245</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
+        <f t="shared" si="0"/>
+        <v>246</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="22">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="22">
+        <f t="shared" si="0"/>
+        <v>249</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="46"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="46"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="30">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="30">
+        <f t="shared" si="0"/>
+        <v>253</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="30">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="46"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+    </row>
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>